<commit_message>
code changes & file 정리
code changes & file 정리
</commit_message>
<xml_diff>
--- a/NetbeansProjects/Parade Route Dynamic Graph/Input All Data Template.xlsx
+++ b/NetbeansProjects/Parade Route Dynamic Graph/Input All Data Template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\Data-Structure-Design\NetbeansProjects\Parade Route Dynamic Graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8C0FCD-6C73-4FEA-9A79-4898DD318265}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A423F26E-EF33-4C4E-8563-E04DE2899321}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11520" xr2:uid="{DB80B1E7-9F7A-4D9D-A4B1-CD69F722C987}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11520" activeTab="1" xr2:uid="{DB80B1E7-9F7A-4D9D-A4B1-CD69F722C987}"/>
   </bookViews>
   <sheets>
-    <sheet name="자료" sheetId="1" r:id="rId1"/>
+    <sheet name="전체 교차로" sheetId="1" r:id="rId1"/>
+    <sheet name="행진 정보" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="104">
   <si>
     <t>교차로</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -104,10 +105,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>영천시장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>정동</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -152,10 +149,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>시의회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>개풍</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -200,10 +193,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>서문관뒤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>세문관</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -316,10 +305,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>세문뒤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>내자</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -361,6 +346,106 @@
   </si>
   <si>
     <t>염천</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>청계광장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대한문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중부, 종로, 남대문 관내 행진 교차로 Template</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.02.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시위대명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신고 인원(명)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>행진 경로(교차로)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새한국</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:40~17:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>청계광장→세종→세문관→광화문→동십자→안국→인사동→종로2→종로1→서린→세종→청계광장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구명총</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:30~17:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세종→서린→종로1→종로2→종로3→종로2→종로1→서린→세종</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태극기국민평의회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한국은행→눈스퀘어→을지1→광교→종로1→서린→세종</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>석방운동본부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:30~19:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울역→남대문→한국은행→눈스퀘어→을지1→광교→종로1→서린→세종→세문관→광화문→세문관</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태극기행동본부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:20~18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세종→세문관→광화문→동십자→안국→인사동→종로2→종로1→서린→세종</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태극기국민운동본부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:30~18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대한문→환구단→개풍→을지1→눈스퀘어→한국은행→남대문→태평→대한문</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -368,7 +453,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +487,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -417,7 +511,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -440,13 +534,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -465,11 +618,44 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68845A3-11EA-453C-8EBA-5F2686C053D6}">
-  <dimension ref="B1:I251"/>
+  <dimension ref="B1:F249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K98" sqref="K98"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N58" sqref="N58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -797,29 +983,24 @@
     <col min="3" max="3" width="11.25" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="6" max="6" width="13.375" customWidth="1"/>
-    <col min="7" max="7" width="11.875" customWidth="1"/>
-    <col min="8" max="8" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+    <row r="1" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="2:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -830,31 +1011,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D5" s="5">
         <v>350</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" s="5">
         <v>310</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>14</v>
@@ -863,100 +1044,100 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="5">
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="5">
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="5">
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D11" s="5">
         <v>260</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D12" s="5">
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="D13" s="5">
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="5">
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="5">
         <v>320</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" s="5">
         <v>290</v>
@@ -964,10 +1145,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="5">
         <v>150</v>
@@ -975,10 +1156,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5">
         <v>440</v>
@@ -986,10 +1167,10 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D19" s="5">
         <v>230</v>
@@ -997,10 +1178,10 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D20" s="5">
         <v>370</v>
@@ -1008,10 +1189,10 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D21" s="5">
         <v>230</v>
@@ -1019,10 +1200,10 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D22" s="5">
         <v>210</v>
@@ -1030,10 +1211,10 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D23" s="5">
         <v>300</v>
@@ -1041,10 +1222,10 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D24" s="5">
         <v>160</v>
@@ -1052,10 +1233,10 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D25" s="5">
         <v>380</v>
@@ -1063,10 +1244,10 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26" s="5">
         <v>230</v>
@@ -1074,10 +1255,10 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D27" s="5">
         <v>220</v>
@@ -1085,10 +1266,10 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D28" s="5">
         <v>260</v>
@@ -1096,10 +1277,10 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D29" s="5">
         <v>140</v>
@@ -1107,10 +1288,10 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D30" s="5">
         <v>310</v>
@@ -1118,10 +1299,10 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D31" s="5">
         <v>440</v>
@@ -1129,10 +1310,10 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="D32" s="5">
         <v>250</v>
@@ -1140,10 +1321,10 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D33" s="5">
         <v>410</v>
@@ -1151,10 +1332,10 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D34" s="5">
         <v>330</v>
@@ -1162,10 +1343,10 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D35" s="5">
         <v>500</v>
@@ -1173,10 +1354,10 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D36" s="5">
         <v>160</v>
@@ -1184,10 +1365,10 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D37" s="5">
         <v>550</v>
@@ -1283,10 +1464,10 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D46" s="5">
         <v>350</v>
@@ -1294,10 +1475,10 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D47" s="5">
         <v>190</v>
@@ -1305,10 +1486,10 @@
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D48" s="5">
         <v>150</v>
@@ -1316,10 +1497,10 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D49" s="3">
         <v>300</v>
@@ -1327,10 +1508,10 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D50" s="5">
         <v>420</v>
@@ -1338,10 +1519,10 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D51" s="5">
         <v>510</v>
@@ -1352,7 +1533,7 @@
         <v>15</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D52" s="5">
         <v>510</v>
@@ -1374,7 +1555,7 @@
         <v>15</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D54" s="5">
         <v>260</v>
@@ -1396,10 +1577,10 @@
         <v>13</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="D56" s="5">
-        <v>330</v>
+        <v>440</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
@@ -1407,10 +1588,10 @@
         <v>13</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D57" s="5">
-        <v>250</v>
+        <v>330</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
@@ -1437,7 +1618,7 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>13</v>
@@ -1448,10 +1629,10 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D61" s="5">
         <v>490</v>
@@ -1459,10 +1640,10 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D62" s="5">
         <v>500</v>
@@ -1470,10 +1651,10 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D63" s="5">
         <v>370</v>
@@ -1481,10 +1662,10 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D64" s="5">
         <v>350</v>
@@ -1492,10 +1673,10 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D65" s="5">
         <v>490</v>
@@ -1503,10 +1684,10 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D66" s="5">
         <v>260</v>
@@ -1514,10 +1695,10 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="D67" s="5">
         <v>90</v>
@@ -1525,10 +1706,10 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D68" s="5">
         <v>220</v>
@@ -1536,10 +1717,10 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B69" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="D69" s="5">
         <v>900</v>
@@ -1547,54 +1728,54 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B70" s="5" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="D70" s="5">
-        <v>390</v>
+        <v>230</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B71" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D71" s="5">
-        <v>230</v>
+        <v>470</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B72" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D72" s="5">
-        <v>470</v>
+        <v>290</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B73" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D73" s="5">
-        <v>290</v>
+        <v>160</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B74" s="5" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D74" s="5">
         <v>160</v>
@@ -1602,288 +1783,288 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D75" s="5">
-        <v>160</v>
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D76" s="5">
-        <v>270</v>
+        <v>190</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D77" s="5">
-        <v>190</v>
+        <v>15</v>
+      </c>
+      <c r="D77" s="3">
+        <v>510</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D78" s="3">
-        <v>510</v>
+        <v>66</v>
+      </c>
+      <c r="D78" s="5">
+        <v>460</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B79" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="D79" s="5">
-        <v>460</v>
+        <v>400</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B80" s="5" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D80" s="5">
-        <v>400</v>
+        <v>460</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B81" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D81" s="5">
-        <v>460</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B82" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D82" s="5">
-        <v>230</v>
+        <v>360</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B83" s="5" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="D83" s="5">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B84" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D84" s="5">
-        <v>350</v>
+        <v>320</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B85" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D85" s="5">
-        <v>320</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B86" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D86" s="5">
-        <v>120</v>
+        <v>190</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B87" s="5" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="D87" s="5">
-        <v>190</v>
+        <v>330</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D88" s="5">
-        <v>330</v>
+        <v>250</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B89" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D89" s="5">
-        <v>250</v>
+        <v>550</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B90" s="5" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="D90" s="5">
-        <v>550</v>
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B91" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D91" s="5">
-        <v>140</v>
+        <v>300</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B92" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D92" s="5">
-        <v>300</v>
+        <v>130</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B93" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D93" s="5">
-        <v>130</v>
+        <v>190</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B94" s="5" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="D94" s="5">
-        <v>190</v>
+        <v>380</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B95" s="5" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="D95" s="5">
-        <v>380</v>
+        <v>470</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B96" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D96" s="5">
-        <v>470</v>
+        <v>460</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B97" s="5" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="D97" s="5">
-        <v>460</v>
+        <v>350</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B98" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D98" s="5">
-        <v>350</v>
+        <v>900</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B99" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C99" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="D99" s="5">
-        <v>900</v>
+        <v>380</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B100" s="5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D100" s="5">
-        <v>380</v>
+        <v>500</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.3">
@@ -1894,392 +2075,392 @@
         <v>18</v>
       </c>
       <c r="D101" s="5">
-        <v>500</v>
+        <v>330</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B102" s="5" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D102" s="5">
-        <v>500</v>
+        <v>310</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B103" s="5" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D103" s="5">
-        <v>330</v>
+        <v>120</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B104" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D104" s="5">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B105" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D105" s="5">
-        <v>120</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B106" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D106" s="5">
-        <v>300</v>
+        <v>320</v>
       </c>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B107" s="5" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D107" s="5">
-        <v>200</v>
+        <v>500</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B108" s="5" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="D108" s="5">
-        <v>320</v>
+        <v>440</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B109" s="5" t="s">
+      <c r="B109" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C109" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D109" s="5">
-        <v>500</v>
+      <c r="C109" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D109" s="3">
+        <v>400</v>
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B110" s="5" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D110" s="5">
-        <v>440</v>
+        <v>190</v>
       </c>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B111" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D111" s="3">
-        <v>400</v>
+      <c r="B111" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" s="5">
+        <v>270</v>
       </c>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B112" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D112" s="5">
-        <v>190</v>
+        <v>380</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B113" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D113" s="5">
-        <v>270</v>
+        <v>50</v>
+      </c>
+      <c r="D113" s="3">
+        <v>370</v>
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B114" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D114" s="5">
-        <v>380</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B115" s="5" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D115" s="3">
+        <v>52</v>
+      </c>
+      <c r="D115" s="5">
         <v>370</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B116" s="5" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D116" s="5">
-        <v>160</v>
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B117" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D117" s="5">
-        <v>370</v>
+        <v>210</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B118" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D118" s="5">
-        <v>130</v>
+        <v>160</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B119" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D119" s="5">
-        <v>210</v>
+        <v>340</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B120" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D120" s="5">
-        <v>160</v>
+        <v>390</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B121" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D121" s="5">
-        <v>340</v>
+        <v>240</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B122" s="5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D122" s="5">
-        <v>390</v>
+        <v>190</v>
       </c>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B123" s="5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D123" s="5">
-        <v>240</v>
+        <v>21</v>
+      </c>
+      <c r="D123" s="3">
+        <v>370</v>
       </c>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B124" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D124" s="5">
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B125" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D125" s="3">
-        <v>370</v>
+        <v>35</v>
+      </c>
+      <c r="D125" s="5">
+        <v>250</v>
       </c>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B126" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D126" s="5">
-        <v>210</v>
+        <v>150</v>
       </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B127" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D127" s="5">
-        <v>250</v>
+        <v>150</v>
       </c>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B128" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="D128" s="5">
-        <v>150</v>
+        <v>510</v>
       </c>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B129" s="5" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D129" s="5">
-        <v>150</v>
+        <v>200</v>
       </c>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B130" s="5" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="D130" s="5">
-        <v>510</v>
+        <v>160</v>
       </c>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B131" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D131" s="5">
-        <v>200</v>
+        <v>250</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B132" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D132" s="5">
-        <v>160</v>
+        <v>120</v>
       </c>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B133" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="D133" s="5">
-        <v>250</v>
+        <v>170</v>
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B134" s="5" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D134" s="5">
-        <v>120</v>
+        <v>380</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B135" s="5" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D135" s="5">
-        <v>170</v>
+        <v>240</v>
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B136" s="5" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="D136" s="5">
-        <v>380</v>
+        <v>220</v>
       </c>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.3">
@@ -2287,10 +2468,10 @@
         <v>12</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D137" s="5">
-        <v>240</v>
+        <v>270</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.3">
@@ -2298,227 +2479,227 @@
         <v>12</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D138" s="5">
-        <v>220</v>
+        <v>140</v>
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B139" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C139" s="5" t="s">
-        <v>16</v>
+        <v>58</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="D139" s="5">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B140" s="5" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D140" s="5">
-        <v>140</v>
+        <v>370</v>
       </c>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B141" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>60</v>
+        <v>45</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D141" s="5">
-        <v>260</v>
+        <v>440</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B142" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D142" s="5">
-        <v>370</v>
+        <v>290</v>
       </c>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B143" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D143" s="5">
-        <v>440</v>
+        <v>330</v>
       </c>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B144" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D144" s="5">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B145" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D145" s="5">
-        <v>330</v>
+        <v>390</v>
       </c>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B146" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D146" s="5">
-        <v>300</v>
+        <v>500</v>
       </c>
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B147" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D147" s="5">
-        <v>390</v>
+        <v>330</v>
       </c>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B148" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D148" s="5">
-        <v>500</v>
+        <v>270</v>
       </c>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B149" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D149" s="5">
-        <v>330</v>
+        <v>350</v>
       </c>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B150" s="5" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D150" s="5">
-        <v>270</v>
+        <v>510</v>
       </c>
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B151" s="5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D151" s="5">
-        <v>350</v>
+        <v>230</v>
       </c>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B152" s="5" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="D152" s="5">
-        <v>510</v>
+        <v>250</v>
       </c>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B153" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D153" s="5">
-        <v>230</v>
+        <v>160</v>
       </c>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B154" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D154" s="5">
-        <v>250</v>
+        <v>190</v>
       </c>
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B155" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D155" s="5">
-        <v>160</v>
+        <v>340</v>
       </c>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B156" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D156" s="5">
-        <v>190</v>
+        <v>300</v>
       </c>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B157" s="5" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="D157" s="5">
-        <v>340</v>
+        <v>300</v>
       </c>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B158" s="5" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="D158" s="5">
         <v>300</v>
@@ -2526,98 +2707,98 @@
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B159" s="5" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D159" s="5">
-        <v>300</v>
+        <v>77</v>
+      </c>
+      <c r="D159" s="3">
+        <v>400</v>
       </c>
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B160" s="5" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="D160" s="5">
-        <v>300</v>
+        <v>260</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B161" s="5" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D161" s="3">
-        <v>400</v>
+        <v>56</v>
+      </c>
+      <c r="D161" s="5">
+        <v>230</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B162" s="5" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="D162" s="5">
-        <v>260</v>
+        <v>310</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B163" s="5" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D163" s="5">
-        <v>230</v>
+        <v>290</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B164" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D164" s="5">
-        <v>310</v>
+        <v>260</v>
       </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B165" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D165" s="5">
-        <v>290</v>
+        <v>420</v>
       </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B166" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D166" s="5">
-        <v>260</v>
+        <v>170</v>
       </c>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B167" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D167" s="5">
         <v>420</v>
@@ -2625,79 +2806,79 @@
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B168" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D168" s="5">
-        <v>170</v>
+        <v>450</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B169" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D169" s="5">
-        <v>420</v>
+        <v>210</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B170" s="5" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D170" s="5">
-        <v>450</v>
+        <v>230</v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B171" s="5" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D171" s="5">
-        <v>210</v>
+        <v>450</v>
       </c>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B172" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D172" s="5">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B173" s="5" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D173" s="5">
-        <v>450</v>
+        <v>500</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B174" s="5" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="D174" s="5">
-        <v>220</v>
+        <v>300</v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.3">
@@ -2705,18 +2886,18 @@
         <v>5</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D175" s="5">
-        <v>500</v>
+        <v>680</v>
       </c>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B176" s="5" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="D176" s="5">
         <v>300</v>
@@ -2724,541 +2905,541 @@
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B177" s="5" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="D177" s="5">
-        <v>680</v>
+        <v>160</v>
       </c>
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B178" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D178" s="5">
-        <v>300</v>
+        <v>390</v>
       </c>
     </row>
     <row r="179" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B179" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="D179" s="5">
-        <v>160</v>
+        <v>340</v>
       </c>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B180" s="5" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="D180" s="5">
-        <v>390</v>
+        <v>510</v>
       </c>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B181" s="5" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D181" s="5">
-        <v>340</v>
+        <v>460</v>
       </c>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B182" s="5" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="D182" s="5">
-        <v>510</v>
+        <v>270</v>
       </c>
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B183" s="5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D183" s="5">
-        <v>460</v>
+        <v>210</v>
       </c>
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B184" s="5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="D184" s="5">
-        <v>270</v>
+        <v>150</v>
       </c>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B185" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D185" s="5">
-        <v>210</v>
+        <v>170</v>
       </c>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B186" s="5" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C186" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D186" s="5">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B187" s="5" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="D187" s="5">
-        <v>170</v>
+        <v>500</v>
       </c>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B188" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D188" s="5">
-        <v>170</v>
+        <v>330</v>
       </c>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B189" s="5" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D189" s="5">
-        <v>500</v>
+        <v>300</v>
       </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B190" s="5" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D190" s="5">
-        <v>330</v>
+        <v>300</v>
       </c>
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B191" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="D191" s="5">
-        <v>300</v>
+        <v>160</v>
       </c>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B192" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D192" s="5">
-        <v>300</v>
+        <v>390</v>
       </c>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B193" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C193" s="5" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D193" s="5">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B194" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D194" s="5">
-        <v>390</v>
+        <v>120</v>
       </c>
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B195" s="5" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C195" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D195" s="5">
-        <v>170</v>
+        <v>200</v>
       </c>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B196" s="5" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D196" s="5">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B197" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D197" s="5">
-        <v>200</v>
+        <v>410</v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B198" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D198" s="5">
-        <v>150</v>
+        <v>320</v>
       </c>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B199" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C199" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D199" s="5">
-        <v>410</v>
+        <v>800</v>
       </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B200" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C200" s="5" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D200" s="5">
-        <v>320</v>
+        <v>550</v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B201" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C201" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D201" s="5">
-        <v>800</v>
+        <v>340</v>
       </c>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B202" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C202" s="5" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="D202" s="5">
-        <v>550</v>
+        <v>800</v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B203" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C203" s="5" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D203" s="5">
-        <v>340</v>
+        <v>390</v>
       </c>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B204" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C204" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D204" s="5">
-        <v>800</v>
+        <v>230</v>
       </c>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B205" s="5" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C205" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D205" s="5">
-        <v>390</v>
+        <v>250</v>
       </c>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B206" s="5" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C206" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D206" s="5">
-        <v>230</v>
+        <v>390</v>
       </c>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B207" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C207" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D207" s="5">
-        <v>250</v>
+        <v>230</v>
       </c>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B208" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C208" s="5" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D208" s="5">
-        <v>390</v>
+        <v>550</v>
       </c>
     </row>
     <row r="209" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B209" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C209" s="5" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D209" s="5">
-        <v>230</v>
+        <v>350</v>
       </c>
     </row>
     <row r="210" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B210" s="5" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C210" s="5" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D210" s="5">
-        <v>550</v>
+        <v>440</v>
       </c>
     </row>
     <row r="211" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B211" s="5" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C211" s="5" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D211" s="5">
-        <v>350</v>
+        <v>210</v>
       </c>
     </row>
     <row r="212" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B212" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C212" s="5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D212" s="5">
-        <v>440</v>
+        <v>230</v>
       </c>
     </row>
     <row r="213" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B213" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C213" s="5" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="D213" s="5">
-        <v>210</v>
+        <v>430</v>
       </c>
     </row>
     <row r="214" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B214" s="5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C214" s="5" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D214" s="5">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="215" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B215" s="5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C215" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D215" s="5">
-        <v>430</v>
+        <v>230</v>
       </c>
     </row>
     <row r="216" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B216" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C216" s="5" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D216" s="5">
-        <v>220</v>
+        <v>430</v>
       </c>
     </row>
     <row r="217" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B217" s="5" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="C217" s="5" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D217" s="5">
-        <v>230</v>
+        <v>440</v>
       </c>
     </row>
     <row r="218" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B218" s="5" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="C218" s="5" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D218" s="5">
-        <v>430</v>
+        <v>260</v>
       </c>
     </row>
     <row r="219" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B219" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C219" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D219" s="5">
-        <v>260</v>
+        <v>190</v>
       </c>
     </row>
     <row r="220" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B220" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C220" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D220" s="5">
-        <v>190</v>
+        <v>130</v>
       </c>
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B221" s="5" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C221" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D221" s="5">
-        <v>130</v>
+        <v>240</v>
       </c>
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B222" s="5" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C222" s="5" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D222" s="5">
-        <v>220</v>
+        <v>150</v>
       </c>
     </row>
     <row r="223" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B223" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C223" s="5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D223" s="5">
-        <v>240</v>
+        <v>120</v>
       </c>
     </row>
     <row r="224" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B224" s="5" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C224" s="5" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="D224" s="5">
-        <v>150</v>
+        <v>420</v>
       </c>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B225" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C225" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D225" s="5">
-        <v>120</v>
+        <v>9</v>
+      </c>
+      <c r="C225" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D225" s="4">
+        <v>110</v>
       </c>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.3">
@@ -3266,21 +3447,21 @@
         <v>9</v>
       </c>
       <c r="C226" s="5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D226" s="5">
-        <v>420</v>
+        <v>220</v>
       </c>
     </row>
     <row r="227" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B227" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C227" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D227" s="4">
-        <v>110</v>
+      <c r="C227" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D227" s="5">
+        <v>680</v>
       </c>
     </row>
     <row r="228" spans="2:4" x14ac:dyDescent="0.3">
@@ -3288,54 +3469,54 @@
         <v>9</v>
       </c>
       <c r="C228" s="5" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="D228" s="5">
-        <v>220</v>
+        <v>370</v>
       </c>
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B229" s="5" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D229" s="5">
-        <v>680</v>
+        <v>420</v>
       </c>
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B230" s="5" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C230" s="5" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D230" s="5">
-        <v>370</v>
+        <v>230</v>
       </c>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B231" s="5" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C231" s="5" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D231" s="5">
-        <v>420</v>
+        <v>600</v>
       </c>
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B232" s="5" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="D232" s="5">
-        <v>230</v>
+        <v>630</v>
       </c>
     </row>
     <row r="233" spans="2:4" x14ac:dyDescent="0.3">
@@ -3343,32 +3524,32 @@
         <v>10</v>
       </c>
       <c r="C233" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D233" s="5">
-        <v>600</v>
+        <v>180</v>
       </c>
     </row>
     <row r="234" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B234" s="5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D234" s="5">
-        <v>630</v>
+        <v>400</v>
       </c>
     </row>
     <row r="235" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B235" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C235" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C235" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D235" s="5">
-        <v>180</v>
+        <v>630</v>
       </c>
     </row>
     <row r="236" spans="2:4" x14ac:dyDescent="0.3">
@@ -3376,29 +3557,29 @@
         <v>17</v>
       </c>
       <c r="C236" s="5" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="D236" s="5">
-        <v>400</v>
+        <v>370</v>
       </c>
     </row>
     <row r="237" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B237" s="5" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="C237" s="5" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="D237" s="5">
-        <v>630</v>
+        <v>360</v>
       </c>
     </row>
     <row r="238" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B238" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C238" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="C238" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="D238" s="5">
         <v>370</v>
@@ -3406,68 +3587,68 @@
     </row>
     <row r="239" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B239" s="5" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="C239" s="5" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="D239" s="5">
-        <v>360</v>
+        <v>230</v>
       </c>
     </row>
     <row r="240" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B240" s="5" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="C240" s="5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D240" s="5">
-        <v>370</v>
+        <v>90</v>
       </c>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B241" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C241" s="5" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D241" s="5">
-        <v>230</v>
+        <v>150</v>
       </c>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B242" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C242" s="5" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D242" s="5">
-        <v>90</v>
+        <v>170</v>
       </c>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B243" s="5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C243" s="5" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D243" s="5">
-        <v>150</v>
+        <v>520</v>
       </c>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B244" s="5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C244" s="5" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D244" s="5">
-        <v>170</v>
+        <v>210</v>
       </c>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.3">
@@ -3475,10 +3656,10 @@
         <v>16</v>
       </c>
       <c r="C245" s="5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D245" s="5">
-        <v>520</v>
+        <v>270</v>
       </c>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.3">
@@ -3486,32 +3667,32 @@
         <v>16</v>
       </c>
       <c r="C246" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D246" s="5">
-        <v>210</v>
+        <v>180</v>
       </c>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B247" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C247" s="5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D247" s="5">
-        <v>270</v>
+        <v>120</v>
       </c>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B248" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C248" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D248" s="5">
-        <v>180</v>
+        <v>130</v>
       </c>
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.3">
@@ -3519,39 +3700,13 @@
         <v>14</v>
       </c>
       <c r="C249" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D249" s="5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B250" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C250" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D250" s="5">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B251" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C251" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D251" s="5">
         <v>140</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B5:D251">
-    <sortCondition ref="B5:B251"/>
-    <sortCondition ref="C5:C251"/>
-  </sortState>
   <mergeCells count="1">
     <mergeCell ref="B2:F2"/>
   </mergeCells>
@@ -3559,4 +3714,159 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0DE4F8-8BAE-4D10-BEE3-BE439C562FDA}">
+  <dimension ref="B1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="18.625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.75" style="6" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="86.25" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.875" style="8" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="2:6" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="2:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B4" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="12">
+        <v>300</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="12">
+        <v>100</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="12">
+        <v>100</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="12">
+        <v>3000</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="12">
+        <v>300</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="12">
+        <v>600</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>